<commit_message>
No Gang Land Update
</commit_message>
<xml_diff>
--- a/Sinner_Stuff/dispatch.xlsx
+++ b/Sinner_Stuff/dispatch.xlsx
@@ -23974,86 +23974,86 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1099001</v>
+        <v>1047001</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Dream Interpretation</t>
+          <t>Bounty Offer</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>夢の解析</t>
+          <t>懸賞依頼</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>꿈의 해석</t>
+          <t>현상금 의뢰</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>梦的解析</t>
+          <t>悬赏委托</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>夢的解析</t>
+          <t>懸賞委託</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+          <t>According to credible leads, a crime boss long pursued by the Public Security Bureau has fled to WhiteSands. With the outlaw's whereabouts unknown, the Bureau decides to secretly issue a huge bounty to recruit a Sinner from WhiteSands for the capture operation.</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+          <t>信頼できる情報提供者によると、治安局が長い間追跡してきた犯罪組織のリーダーが砂の海に逃亡したという。その後の行方が掴めていないため、治安局は密かに高額な懸賞金をかけて、砂の海出身のコンビクトに協力依頼を出した。</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+          <t>믿을만한 소식에 따르면, 치안국에서 오랫동안 추적해 온 범죄 조직의 두목이 화이트 샌드로 도주했다고 한다. 행방이 묘연한 가운데 치안국은 비밀리에 고액 현상금을 내걸고 화이트 샌드 현지의 수감자를 모집해 검거에 나서고자 한다.</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+          <t>据可靠线报表示，治安局追查已久的犯罪团伙头目已逃往砂海，因其行踪成谜，治安局决定秘密发布高额悬赏，招募一位砂海本地的禁闭者参与抓捕。</t>
         </is>
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+          <t>據可靠線報表示，治安局追查已久的犯罪集團頭目已逃往砂海，因其行蹤成謎，治安局決定秘密發布高額懸賞，招募一位砂海本地的禁閉者參與抓捕。</t>
         </is>
       </c>
       <c r="M152" t="inlineStr">
         <is>
-          <t>Hecate</t>
+          <t>Korryn</t>
         </is>
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>ヘカテー</t>
+          <t>コリン</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
         <is>
-          <t>헤카테</t>
+          <t>코린</t>
         </is>
       </c>
       <c r="P152" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>柯琳</t>
         </is>
       </c>
       <c r="Q152" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>柯琳</t>
         </is>
       </c>
       <c r="R152" t="inlineStr"/>
@@ -24063,60 +24063,530 @@
       <c r="V152" t="inlineStr"/>
       <c r="W152" t="inlineStr">
         <is>
+          <t>Bronze Crystal</t>
+        </is>
+      </c>
+      <c r="X152" t="inlineStr">
+        <is>
+          <t>曲銅結晶</t>
+        </is>
+      </c>
+      <c r="Y152" t="inlineStr">
+        <is>
+          <t>곡선형 구리 결정</t>
+        </is>
+      </c>
+      <c r="Z152" t="inlineStr">
+        <is>
+          <t>曲铜晶</t>
+        </is>
+      </c>
+      <c r="AA152" t="inlineStr">
+        <is>
+          <t>曲銅晶</t>
+        </is>
+      </c>
+      <c r="AB152" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC152" t="inlineStr">
+        <is>
+          <t>Bronze Concentrate</t>
+        </is>
+      </c>
+      <c r="AD152" t="inlineStr">
+        <is>
+          <t>曲銅の精鉱</t>
+        </is>
+      </c>
+      <c r="AE152" t="inlineStr">
+        <is>
+          <t>정교한 곡선형 구리 광석</t>
+        </is>
+      </c>
+      <c r="AF152" t="inlineStr">
+        <is>
+          <t>曲铜精矿</t>
+        </is>
+      </c>
+      <c r="AG152" t="inlineStr">
+        <is>
+          <t>曲銅精礦</t>
+        </is>
+      </c>
+      <c r="AH152" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>1047002</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Seasoned Mediator</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>調停専門家</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>중재 전문가</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>调停专家</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>調停專家</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>A violent dispute due to sales competition has broken out between two neighboring businesses on an Eastside shopping street. An experienced mediator with business management knowledge is urgently required to prevent further property damage from the escalating situation.</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>ニューシティの歩道で、隣接する二つの店舗が激しく争っている。原因は店舗間の競争の激化だ。暴力による財産の損害を軽減するため、経営と紛争調停に精通した人材を緊急派遣する必要がある。</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>신성의 한 보행자 거리에 인접해 있는 두 점포 간에 과열된 경쟁과 갈등으로 인한 싸움이 일어났다. 경영과 중재에 능한 사람을 조속히 파견해 폭행 사건으로 인한 재산 피해를 최대한 줄여야 한다.</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>新城某步行街，两处相邻店家发生激烈争执大打出手，起因为店铺之间的竞争与冲突，需要紧急派遣一位熟悉经营与冲突调停的人员，减少因暴力事件引起的财物损毁。</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>新城某步行街，兩處相鄰店家發生激烈爭執大打出手，起因為店舖之間的競爭與衝突，需要緊急派遣一位熟悉經營與衝突調停的人員，減少因暴力事件引起的財物損毀。</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>Mira</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>ミラ</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>미라</t>
+        </is>
+      </c>
+      <c r="P153" t="inlineStr">
+        <is>
+          <t>米拉</t>
+        </is>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>米拉</t>
+        </is>
+      </c>
+      <c r="R153" t="inlineStr"/>
+      <c r="S153" t="inlineStr"/>
+      <c r="T153" t="inlineStr"/>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>Bronze Concentrate</t>
+        </is>
+      </c>
+      <c r="X153" t="inlineStr">
+        <is>
+          <t>曲銅の精鉱</t>
+        </is>
+      </c>
+      <c r="Y153" t="inlineStr">
+        <is>
+          <t>정교한 곡선형 구리 광석</t>
+        </is>
+      </c>
+      <c r="Z153" t="inlineStr">
+        <is>
+          <t>曲铜精矿</t>
+        </is>
+      </c>
+      <c r="AA153" t="inlineStr">
+        <is>
+          <t>曲銅精礦</t>
+        </is>
+      </c>
+      <c r="AB153" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC153" t="inlineStr">
+        <is>
+          <t>Bronze Raw Ore</t>
+        </is>
+      </c>
+      <c r="AD153" t="inlineStr">
+        <is>
+          <t>曲銅の原鉱</t>
+        </is>
+      </c>
+      <c r="AE153" t="inlineStr">
+        <is>
+          <t>거친 곡선형 구리 광석</t>
+        </is>
+      </c>
+      <c r="AF153" t="inlineStr">
+        <is>
+          <t>曲铜粗矿</t>
+        </is>
+      </c>
+      <c r="AG153" t="inlineStr">
+        <is>
+          <t>曲銅粗礦</t>
+        </is>
+      </c>
+      <c r="AH153" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>1047003</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Management Expert</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>経営管理の人材</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>경영관리 인재</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>管理人才</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>管理人才</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>The Public Security Bureau's new creative merchandise has hit its lowest sales record and is making severe losses. An experienced management expert is required to provide business consultation.</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>治安局が新たに開発した文化的なオリジナルグッズの売り上げが過去最低を記録し、損失も深刻だ。管理と経営に精通した優秀な人材の指導が急務となっている。</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>치안국에서 새로 기획한 굿즈의 판매량이 사상 최저치를 기록해 심각한 손실이 발생했다. 경영관리 능력을 갖춘 인재를 조속히 파견해 지도해야 한다.</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>治安局新研发的文创产品销量创史低，亏损严重，急需熟悉管理与经营的优秀人才前去指导。</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>治安局新研發的文創產品銷量創史低，虧損嚴重，急需熟悉管理與經營的優秀人才前去指導。</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>Mira</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>ミラ</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>미라</t>
+        </is>
+      </c>
+      <c r="P154" t="inlineStr">
+        <is>
+          <t>米拉</t>
+        </is>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>米拉</t>
+        </is>
+      </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>Rise</t>
+        </is>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>ライズ</t>
+        </is>
+      </c>
+      <c r="T154" t="inlineStr">
+        <is>
+          <t>라이즈</t>
+        </is>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>瑞思</t>
+        </is>
+      </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>瑞思</t>
+        </is>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>Bronze Concentrate</t>
+        </is>
+      </c>
+      <c r="X154" t="inlineStr">
+        <is>
+          <t>曲銅の精鉱</t>
+        </is>
+      </c>
+      <c r="Y154" t="inlineStr">
+        <is>
+          <t>정교한 곡선형 구리 광석</t>
+        </is>
+      </c>
+      <c r="Z154" t="inlineStr">
+        <is>
+          <t>曲铜精矿</t>
+        </is>
+      </c>
+      <c r="AA154" t="inlineStr">
+        <is>
+          <t>曲銅精礦</t>
+        </is>
+      </c>
+      <c r="AB154" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC154" t="inlineStr">
+        <is>
+          <t>Bronze Concentrate</t>
+        </is>
+      </c>
+      <c r="AD154" t="inlineStr">
+        <is>
+          <t>曲銅の精鉱</t>
+        </is>
+      </c>
+      <c r="AE154" t="inlineStr">
+        <is>
+          <t>정교한 곡선형 구리 광석</t>
+        </is>
+      </c>
+      <c r="AF154" t="inlineStr">
+        <is>
+          <t>曲铜精矿</t>
+        </is>
+      </c>
+      <c r="AG154" t="inlineStr">
+        <is>
+          <t>曲銅精礦</t>
+        </is>
+      </c>
+      <c r="AH154" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>1099001</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Dream Interpretation</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>夢の解析</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>꿈의 해석</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>梦的解析</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>夢的解析</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>Hecate</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>ヘカテー</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>헤카테</t>
+        </is>
+      </c>
+      <c r="P155" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="R155" t="inlineStr"/>
+      <c r="S155" t="inlineStr"/>
+      <c r="T155" t="inlineStr"/>
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="inlineStr"/>
+      <c r="W155" t="inlineStr">
+        <is>
           <t>Arsenopyrite Concentrate</t>
         </is>
       </c>
-      <c r="X152" t="inlineStr">
+      <c r="X155" t="inlineStr">
         <is>
           <t>毒砂の精鉱</t>
         </is>
       </c>
-      <c r="Y152" t="inlineStr">
+      <c r="Y155" t="inlineStr">
         <is>
           <t>정교한 독모래 광석</t>
         </is>
       </c>
-      <c r="Z152" t="inlineStr">
+      <c r="Z155" t="inlineStr">
         <is>
           <t>毒砂精矿</t>
         </is>
       </c>
-      <c r="AA152" t="inlineStr">
+      <c r="AA155" t="inlineStr">
         <is>
           <t>毒砂精礦</t>
         </is>
       </c>
-      <c r="AB152" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="AC152" t="inlineStr">
+      <c r="AB155" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC155" t="inlineStr">
         <is>
           <t>Arsenopyrite Raw Ore</t>
         </is>
       </c>
-      <c r="AD152" t="inlineStr">
+      <c r="AD155" t="inlineStr">
         <is>
           <t>毒砂の原鉱</t>
         </is>
       </c>
-      <c r="AE152" t="inlineStr">
+      <c r="AE155" t="inlineStr">
         <is>
           <t>거친 독모래 광석</t>
         </is>
       </c>
-      <c r="AF152" t="inlineStr">
+      <c r="AF155" t="inlineStr">
         <is>
           <t>毒砂粗矿</t>
         </is>
       </c>
-      <c r="AG152" t="inlineStr">
+      <c r="AG155" t="inlineStr">
         <is>
           <t>毒砂粗礦</t>
         </is>
       </c>
-      <c r="AH152" t="inlineStr">
+      <c r="AH155" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>

</xml_diff>

<commit_message>
2.5 GLB Anni Updates
</commit_message>
<xml_diff>
--- a/Sinner_Stuff/dispatch.xlsx
+++ b/Sinner_Stuff/dispatch.xlsx
@@ -25854,86 +25854,86 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1099001</v>
+        <v>1051001</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Dream Interpretation</t>
+          <t>Expert at Work</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>夢の解析</t>
+          <t>専門に合った仕事</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>꿈의 해석</t>
+          <t>전문가</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>梦的解析</t>
+          <t>专业对口</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>夢的解析</t>
+          <t>專業對口</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+          <t>The FAC has detected an abnormal rise in M-value at a high school in Eastside. Preliminary investigation reveals that its students have been holding spooky tale-telling séances after school. A request has been submitted to the Bureau to dispatch a suitable Sinner to assist in uncovering the truth.</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+          <t>FACはニューシティのとある高校でM値が異常に上昇していることを検出した。初動調査の結果、その学校の生徒たちの間で、放課後の心霊話会が流行していることが判明した。そのため、真相を探るのに適切なコンビクトを派遣するよう管理局に依頼が来た。</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+          <t>FAC 관측 결과 신성의 모 학교 내에서 M 수치가 비정상적으로 상승했다고 한다. 조사를 진행해 보니 해당 학교의 학생들 사이에서 서로 신비한 이야기를 나누는 방과후 활동이 유행하고 있다고 한다. FAC는 특별히 관리국에 적합한 수감자를 파견해 진상조사를 도와 달라고 요청했다.</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
         <is>
-          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+          <t>FAC监测到新城某高校内M值异常上升，初步调查得知，该校学生间正流行着举办通灵故事会的课后活动，特向管理局申请派一位合适的禁闭者协助探查真相。</t>
         </is>
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+          <t>FAC監測到新城某高校內M值異常上升，初步調查得知，該校學生間正流行著舉辦通靈故事會的課後活動，特向管理局申請派一位合適的禁閉者協助探查真相。</t>
         </is>
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>Hecate</t>
+          <t>Yugu</t>
         </is>
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>ヘカテー</t>
+          <t>玉骨</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
         <is>
-          <t>헤카테</t>
+          <t>유구</t>
         </is>
       </c>
       <c r="P164" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>玉骨</t>
         </is>
       </c>
       <c r="Q164" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>玉骨</t>
         </is>
       </c>
       <c r="R164" t="inlineStr"/>
@@ -25943,60 +25943,680 @@
       <c r="V164" t="inlineStr"/>
       <c r="W164" t="inlineStr">
         <is>
+          <t>Infected Gel</t>
+        </is>
+      </c>
+      <c r="X164" t="inlineStr">
+        <is>
+          <t>感染されたゲル</t>
+        </is>
+      </c>
+      <c r="Y164" t="inlineStr">
+        <is>
+          <t>감염된 젤라틴</t>
+        </is>
+      </c>
+      <c r="Z164" t="inlineStr">
+        <is>
+          <t>感染凝胶</t>
+        </is>
+      </c>
+      <c r="AA164" t="inlineStr">
+        <is>
+          <t>感染凝膠</t>
+        </is>
+      </c>
+      <c r="AB164" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC164" t="inlineStr">
+        <is>
+          <t>Organic Gel</t>
+        </is>
+      </c>
+      <c r="AD164" t="inlineStr">
+        <is>
+          <t>原生ゲル</t>
+        </is>
+      </c>
+      <c r="AE164" t="inlineStr">
+        <is>
+          <t>원시적 젤라틴</t>
+        </is>
+      </c>
+      <c r="AF164" t="inlineStr">
+        <is>
+          <t>原生凝胶</t>
+        </is>
+      </c>
+      <c r="AG164" t="inlineStr">
+        <is>
+          <t>原生凝膠</t>
+        </is>
+      </c>
+      <c r="AH164" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>1051002</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Heaven-Sent Karma</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>天からの功徳</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>하늘이 내린 공덕</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>天降功德</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>天降功德</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>The season is changing and flu outbreaks have emerged across regions. Recognizing this as a heaven-sent opportunity to accumulate good karma, a certain Sinner has eagerly requested permission to go out and provide free medical services.</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>季節の変わり目に、多くの地域でインフルエンザが流行している。これが天からの功徳であると気付いたあるコンビクトは、外出して無料診察を行うことを強く希望した。</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>환절기가 되면 여러 지역에서 유행성 감기가 발발하는데, 이를 하늘이 내린 공덕으로 여긴 한 수감자가 자선 의료 활동을 할 수 있도록 외출을 허가해달라고 강력히 요구했다.</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>季节交替，多地爆发流感，意识到这是天降的功德，某位禁闭者强烈要求外出义诊。</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>季節交替，多地爆發流感，意識到這是天降的功德，某位禁閉者強烈要求外出義診。</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>Wuhuanzi</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>無患子</t>
+        </is>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>무환자</t>
+        </is>
+      </c>
+      <c r="P165" t="inlineStr">
+        <is>
+          <t>无患子</t>
+        </is>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>無患子</t>
+        </is>
+      </c>
+      <c r="R165" t="inlineStr"/>
+      <c r="S165" t="inlineStr"/>
+      <c r="T165" t="inlineStr"/>
+      <c r="U165" t="inlineStr"/>
+      <c r="V165" t="inlineStr"/>
+      <c r="W165" t="inlineStr">
+        <is>
+          <t>Organic Gel</t>
+        </is>
+      </c>
+      <c r="X165" t="inlineStr">
+        <is>
+          <t>原生ゲル</t>
+        </is>
+      </c>
+      <c r="Y165" t="inlineStr">
+        <is>
+          <t>원시적 젤라틴</t>
+        </is>
+      </c>
+      <c r="Z165" t="inlineStr">
+        <is>
+          <t>原生凝胶</t>
+        </is>
+      </c>
+      <c r="AA165" t="inlineStr">
+        <is>
+          <t>原生凝膠</t>
+        </is>
+      </c>
+      <c r="AB165" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC165" t="inlineStr">
+        <is>
+          <t>Condense Gel</t>
+        </is>
+      </c>
+      <c r="AD165" t="inlineStr">
+        <is>
+          <t>懸濁ゲル</t>
+        </is>
+      </c>
+      <c r="AE165" t="inlineStr">
+        <is>
+          <t>현탁 젤라틴</t>
+        </is>
+      </c>
+      <c r="AF165" t="inlineStr">
+        <is>
+          <t>悬浊凝胶</t>
+        </is>
+      </c>
+      <c r="AG165" t="inlineStr">
+        <is>
+          <t>懸濁凝膠</t>
+        </is>
+      </c>
+      <c r="AH165" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>1051003</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Private Bodyguard</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>同行する用心棒</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>수행 경호원</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>随行保镖</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>隨行保鑣</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>SALVA has extended an invitation to discuss traditional Eastian medicine with a certain Sinner. As this Sinner is not a local, company of another Sinner of similar age who is familiar with the route from the Bureau to Syndicate is required.</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>あるコンビクトと東洲の現地医術について学術的な討論をしたいと、彼岸から招待状が届いた。しかし、そのコンビクトはディスの人間ではないため、管理局からシンジケートまでのルートに詳しく、年齢も近いコンビクトに同行してもらう必要がある。</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>구원 병원에서 동방 대륙 본토 의술에 관해 특정 수감자와 함께 학술적인 연구를 진행하길 희망한다며 초대장을 보내왔다. 해당 수감자가 신디케이트 사람이 아니기에 관리국에서 신디케이트로 향하는 길에 익숙한 또래 나이의 수감자를 함께 파견해야 한다.</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>彼岸发来邀请，希望能与某位禁闭者就东洲本土医术进行学术探讨，鉴于该禁闭者非本地人，需要一位熟悉从管理局到辛迪加路线且年龄相仿的禁闭者陪同上路。</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>彼岸發來邀請，希望能與某位禁閉者就東洲本土醫術進行學術探討，鑒於該禁閉者非本地人，需要一位熟悉從管理局到辛迪加路線且年齡相仿的禁閉者陪同上路。</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>Wuhuanzi</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>無患子</t>
+        </is>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>무환자</t>
+        </is>
+      </c>
+      <c r="P166" t="inlineStr">
+        <is>
+          <t>无患子</t>
+        </is>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>無患子</t>
+        </is>
+      </c>
+      <c r="R166" t="inlineStr">
+        <is>
+          <t>Dolly</t>
+        </is>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>ドリー</t>
+        </is>
+      </c>
+      <c r="T166" t="inlineStr">
+        <is>
+          <t>돌리</t>
+        </is>
+      </c>
+      <c r="U166" t="inlineStr">
+        <is>
+          <t>多莉</t>
+        </is>
+      </c>
+      <c r="V166" t="inlineStr">
+        <is>
+          <t>多莉</t>
+        </is>
+      </c>
+      <c r="W166" t="inlineStr">
+        <is>
+          <t>Organic Gel</t>
+        </is>
+      </c>
+      <c r="X166" t="inlineStr">
+        <is>
+          <t>原生ゲル</t>
+        </is>
+      </c>
+      <c r="Y166" t="inlineStr">
+        <is>
+          <t>원시적 젤라틴</t>
+        </is>
+      </c>
+      <c r="Z166" t="inlineStr">
+        <is>
+          <t>原生凝胶</t>
+        </is>
+      </c>
+      <c r="AA166" t="inlineStr">
+        <is>
+          <t>原生凝膠</t>
+        </is>
+      </c>
+      <c r="AB166" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC166" t="inlineStr">
+        <is>
+          <t>Organic Gel</t>
+        </is>
+      </c>
+      <c r="AD166" t="inlineStr">
+        <is>
+          <t>原生ゲル</t>
+        </is>
+      </c>
+      <c r="AE166" t="inlineStr">
+        <is>
+          <t>원시적 젤라틴</t>
+        </is>
+      </c>
+      <c r="AF166" t="inlineStr">
+        <is>
+          <t>原生凝胶</t>
+        </is>
+      </c>
+      <c r="AG166" t="inlineStr">
+        <is>
+          <t>原生凝膠</t>
+        </is>
+      </c>
+      <c r="AH166" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>1051004</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Parade Fairy</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>フロートキャラクター</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>퍼레이드 캐릭터</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>花车仙子</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>花車仙子</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>The Public Security Bureau has received an arson threat targeting an amusement park. The sender is suspected of possessing Mania weapons. A Sinner skilled in creating illusions is urgently required to go undercover as a fairy at the parade and assist the Public Security Bureau in controlling the situation while guiding visitors to safety.</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>治安局に遊園地への放火予告の手紙が届いた。送り主は狂瞳武器を所持している疑いがあり、幻術に長けたコンビクトにフロートに乗ったキャラクターに変装してもらい、治安局と協力して現場を制御し、来場客を安全な場所へ誘導する必要がある。</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>치안국에 놀이공원 방화를 예고하는 편지 한 통이 전달되었다. 편지를 보낸 이는 변이 무기를 소지한 것으로 추측된다. 이에 환술에 능한 수감자를 급히 파견해 퍼레이드 캐릭터로 분장시키고, 치안국을 도와 상황을 통제하며 관광객을 안전한 구역으로 피신시키려 한다.</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>治安局收到一封游乐园纵火预告信，发信人疑似持有狂厄武器，急需一位精通幻术的禁闭者扮成花车仙子，协助治安局控制局面并将游客引导至安全地带。</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>治安局收到一封遊樂園縱火預告信，發信人疑似持有狂厄武器，急需一位精通幻術的禁閉者扮成花車仙子，協助治安局控制局面並將遊客引導至安全地帶。</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>Yingying</t>
+        </is>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>インイン</t>
+        </is>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>잉잉</t>
+        </is>
+      </c>
+      <c r="P167" t="inlineStr">
+        <is>
+          <t>萦萦</t>
+        </is>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>縈縈</t>
+        </is>
+      </c>
+      <c r="R167" t="inlineStr"/>
+      <c r="S167" t="inlineStr"/>
+      <c r="T167" t="inlineStr"/>
+      <c r="U167" t="inlineStr"/>
+      <c r="V167" t="inlineStr"/>
+      <c r="W167" t="inlineStr">
+        <is>
+          <t>Infected Cyst</t>
+        </is>
+      </c>
+      <c r="X167" t="inlineStr">
+        <is>
+          <t>感染された嚢胞</t>
+        </is>
+      </c>
+      <c r="Y167" t="inlineStr">
+        <is>
+          <t>감염된 낭포</t>
+        </is>
+      </c>
+      <c r="Z167" t="inlineStr">
+        <is>
+          <t>感染囊胞</t>
+        </is>
+      </c>
+      <c r="AA167" t="inlineStr">
+        <is>
+          <t>感染囊胞</t>
+        </is>
+      </c>
+      <c r="AB167" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC167" t="inlineStr">
+        <is>
+          <t>Organic Cyst</t>
+        </is>
+      </c>
+      <c r="AD167" t="inlineStr">
+        <is>
+          <t>原生嚢胞</t>
+        </is>
+      </c>
+      <c r="AE167" t="inlineStr">
+        <is>
+          <t>원시적 낭포</t>
+        </is>
+      </c>
+      <c r="AF167" t="inlineStr">
+        <is>
+          <t>原生囊胞</t>
+        </is>
+      </c>
+      <c r="AG167" t="inlineStr">
+        <is>
+          <t>原生囊胞</t>
+        </is>
+      </c>
+      <c r="AH167" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>1099001</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Dream Interpretation</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>夢の解析</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>꿈의 해석</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>梦的解析</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>夢的解析</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>Hecate</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>ヘカテー</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>헤카테</t>
+        </is>
+      </c>
+      <c r="P168" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="R168" t="inlineStr"/>
+      <c r="S168" t="inlineStr"/>
+      <c r="T168" t="inlineStr"/>
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" t="inlineStr"/>
+      <c r="W168" t="inlineStr">
+        <is>
           <t>Arsenopyrite Concentrate</t>
         </is>
       </c>
-      <c r="X164" t="inlineStr">
+      <c r="X168" t="inlineStr">
         <is>
           <t>毒砂の精鉱</t>
         </is>
       </c>
-      <c r="Y164" t="inlineStr">
+      <c r="Y168" t="inlineStr">
         <is>
           <t>정교한 독모래 광석</t>
         </is>
       </c>
-      <c r="Z164" t="inlineStr">
+      <c r="Z168" t="inlineStr">
         <is>
           <t>毒砂精矿</t>
         </is>
       </c>
-      <c r="AA164" t="inlineStr">
+      <c r="AA168" t="inlineStr">
         <is>
           <t>毒砂精礦</t>
         </is>
       </c>
-      <c r="AB164" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="AC164" t="inlineStr">
+      <c r="AB168" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC168" t="inlineStr">
         <is>
           <t>Arsenopyrite Raw Ore</t>
         </is>
       </c>
-      <c r="AD164" t="inlineStr">
+      <c r="AD168" t="inlineStr">
         <is>
           <t>毒砂の原鉱</t>
         </is>
       </c>
-      <c r="AE164" t="inlineStr">
+      <c r="AE168" t="inlineStr">
         <is>
           <t>거친 독모래 광석</t>
         </is>
       </c>
-      <c r="AF164" t="inlineStr">
+      <c r="AF168" t="inlineStr">
         <is>
           <t>毒砂粗矿</t>
         </is>
       </c>
-      <c r="AG164" t="inlineStr">
+      <c r="AG168" t="inlineStr">
         <is>
           <t>毒砂粗礦</t>
         </is>
       </c>
-      <c r="AH164" t="inlineStr">
+      <c r="AH168" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>

</xml_diff>

<commit_message>
GLB - 20250525 Update
</commit_message>
<xml_diff>
--- a/Sinner_Stuff/dispatch.xlsx
+++ b/Sinner_Stuff/dispatch.xlsx
@@ -26474,86 +26474,86 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1099001</v>
+        <v>1052001</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Dream Interpretation</t>
+          <t>Unconventional Wedding</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>夢の解析</t>
+          <t>ニッチな結婚式</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>꿈의 해석</t>
+          <t>독특한 결혼식</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>梦的解析</t>
+          <t>小众婚礼</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>夢的解析</t>
+          <t>小眾婚禮</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+          <t>A rich heiress from Eastside known for her unconventional hobbies has recently gotten engaged and is planning a paranormal-themed wedding. This has caused many wedding planners to back away from the project. When the news reaches the Bureau, a certain Sinner seems very intrigued.</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+          <t>ニューシティのとある名家の令嬢は、ニッチな趣味を持つことで知られている。彼女は最近婚約したばかりで、幽霊をテーマにした結婚式を希望しており、多くのウェディングプランナーが尻込みしている。その噂が管理局に届くと、あるコンビクトが強い関心を示した。</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+          <t>신성의 어느 귀족 집안 아가씨는 독특한 취미로 이름이 높았다. 최근 약혼한 그녀는 오컬트 테마의 결혼식을 원했고, 이는 수많은 웨딩 플래너들을 난처하게 했다. 이 소식을 들은 한 수감자가 큰 흥미를 보였다.</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+          <t>新城某贵族千金以爱好小众而闻名，她刚刚订婚，计划为自己办一场灵异主题的婚礼，这叫许多婚礼策划人望而却步。消息传到管理局，某位禁闭者表现出了不小的兴趣。</t>
         </is>
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+          <t>新城某貴族千金以愛好小眾而聞名，她剛剛訂婚，計畫為自己辦一場靈異主題的婚禮，這叫許多婚禮企劃人望而卻步。消息傳到管理局，某位禁閉者表現出了不小的興趣。</t>
         </is>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>Hecate</t>
+          <t>Graves</t>
         </is>
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>ヘカテー</t>
+          <t>グレイヴ</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
         <is>
-          <t>헤카테</t>
+          <t>그레이브</t>
         </is>
       </c>
       <c r="P168" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>格芮芙</t>
         </is>
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>格芮芙</t>
         </is>
       </c>
       <c r="R168" t="inlineStr"/>
@@ -26563,60 +26563,530 @@
       <c r="V168" t="inlineStr"/>
       <c r="W168" t="inlineStr">
         <is>
+          <t>Infected Elytra</t>
+        </is>
+      </c>
+      <c r="X168" t="inlineStr">
+        <is>
+          <t>感染鞘翅</t>
+        </is>
+      </c>
+      <c r="Y168" t="inlineStr">
+        <is>
+          <t>오염된 겉날개</t>
+        </is>
+      </c>
+      <c r="Z168" t="inlineStr">
+        <is>
+          <t>感染鞘翅</t>
+        </is>
+      </c>
+      <c r="AA168" t="inlineStr">
+        <is>
+          <t>感染鞘翅</t>
+        </is>
+      </c>
+      <c r="AB168" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC168" t="inlineStr">
+        <is>
+          <t>Organic Elytra</t>
+        </is>
+      </c>
+      <c r="AD168" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AE168" t="inlineStr">
+        <is>
+          <t>원시적 겉날개</t>
+        </is>
+      </c>
+      <c r="AF168" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AG168" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AH168" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>1052002</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Home Makeover</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>住宅改造</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>주택 개조</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>房屋改造</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>房屋改造</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>A real estate company has several haunted houses they simply can't sell off, no matter what they try. They're willing to pay a high price for someone to help resolve this desperate situation. Upon hearing this, a certain Sinner eagerly volunteers.</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>ある不動産会社が、なかなか売れない事故物件を複数抱えており、高額な報酬で対応できる人材を探している。それを聞いたあるコンビクトが積極的に参加を申し出た。</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>한 부동산 업체가 여러 개의 흉가 매물을 가지고 있었는데, 아무리 노력해도 팔리지 않아 흉가 매물을 처리해 주는 사람에게 후한 보상을 주겠다고 약속했다. 이 소식을 들은 한 수감자가 적극적으로 이에 지원했다.</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>某房地产公司手头有好几间凶宅，无论如何也抛售不出，希望有人能为他们解决燃眉之急，奖金丰厚。某禁闭者听说后积极要求参与。</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>某房地產公司手頭有好幾間凶宅，無論如何也拋售不出，希望有人能為他們解決燃眉之急，獎金豐厚。某禁閉者聽說後積極要求參與。</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>Luminita</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>ルミニタ</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>루미니타</t>
+        </is>
+      </c>
+      <c r="P169" t="inlineStr">
+        <is>
+          <t>卢米尼塔</t>
+        </is>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>盧米尼塔</t>
+        </is>
+      </c>
+      <c r="R169" t="inlineStr"/>
+      <c r="S169" t="inlineStr"/>
+      <c r="T169" t="inlineStr"/>
+      <c r="U169" t="inlineStr"/>
+      <c r="V169" t="inlineStr"/>
+      <c r="W169" t="inlineStr">
+        <is>
+          <t>Organic Elytra</t>
+        </is>
+      </c>
+      <c r="X169" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="Y169" t="inlineStr">
+        <is>
+          <t>원시적 겉날개</t>
+        </is>
+      </c>
+      <c r="Z169" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AA169" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AB169" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC169" t="inlineStr">
+        <is>
+          <t>Elytra Shard</t>
+        </is>
+      </c>
+      <c r="AD169" t="inlineStr">
+        <is>
+          <t>鞘翅の破片</t>
+        </is>
+      </c>
+      <c r="AE169" t="inlineStr">
+        <is>
+          <t>겉날개 파편</t>
+        </is>
+      </c>
+      <c r="AF169" t="inlineStr">
+        <is>
+          <t>鞘翅残片</t>
+        </is>
+      </c>
+      <c r="AG169" t="inlineStr">
+        <is>
+          <t>鞘翅殘片</t>
+        </is>
+      </c>
+      <c r="AH169" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>1052003</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Dis Haunt</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>戦慄の映画製作</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>공포 전문가</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>月光光心慌慌</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>月光光心慌慌</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>A prominent Eastside director has just announced a new horror film project. They are now urgently recruiting consultants savvy in paranormal phenomena to join the crew.</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>最近、ニューシティのとある有名監督の最新ホラー映画が準備段階の初期に入ったと発表された。現在、撮影協力として霊的分野の専門アドバイザーを多数急募している。</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>최근 신성의 한 유명 감독이 차기 공포 영화 제작을 공식 발표했고 현재 기괴한 현상에 대해 잘 알고 있는 전문가를 급히 모집하고 있다.</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>近日，新城某知名导演的最新恐怖大片宣布进入早期筹备阶段，现正急招多名灵异方面的专业顾问协助拍摄。</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>近日，新城某知名導演的最新恐怖大片宣佈進入早期籌備階段，現正急招多名靈異方面的專業顧問協助拍攝。</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>Luminita</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>ルミニタ</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>루미니타</t>
+        </is>
+      </c>
+      <c r="P170" t="inlineStr">
+        <is>
+          <t>卢米尼塔</t>
+        </is>
+      </c>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>盧米尼塔</t>
+        </is>
+      </c>
+      <c r="R170" t="inlineStr">
+        <is>
+          <t>Letta</t>
+        </is>
+      </c>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>レタ</t>
+        </is>
+      </c>
+      <c r="T170" t="inlineStr">
+        <is>
+          <t>레타</t>
+        </is>
+      </c>
+      <c r="U170" t="inlineStr">
+        <is>
+          <t>莱塔</t>
+        </is>
+      </c>
+      <c r="V170" t="inlineStr">
+        <is>
+          <t>萊塔</t>
+        </is>
+      </c>
+      <c r="W170" t="inlineStr">
+        <is>
+          <t>Organic Elytra</t>
+        </is>
+      </c>
+      <c r="X170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="Y170" t="inlineStr">
+        <is>
+          <t>원시적 겉날개</t>
+        </is>
+      </c>
+      <c r="Z170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AA170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AB170" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC170" t="inlineStr">
+        <is>
+          <t>Organic Elytra</t>
+        </is>
+      </c>
+      <c r="AD170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AE170" t="inlineStr">
+        <is>
+          <t>원시적 겉날개</t>
+        </is>
+      </c>
+      <c r="AF170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AG170" t="inlineStr">
+        <is>
+          <t>原生鞘翅</t>
+        </is>
+      </c>
+      <c r="AH170" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>1099001</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Dream Interpretation</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>夢の解析</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>꿈의 해석</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>梦的解析</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>夢的解析</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>Hecate</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>ヘカテー</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>헤카테</t>
+        </is>
+      </c>
+      <c r="P171" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="R171" t="inlineStr"/>
+      <c r="S171" t="inlineStr"/>
+      <c r="T171" t="inlineStr"/>
+      <c r="U171" t="inlineStr"/>
+      <c r="V171" t="inlineStr"/>
+      <c r="W171" t="inlineStr">
+        <is>
           <t>Arsenopyrite Concentrate</t>
         </is>
       </c>
-      <c r="X168" t="inlineStr">
+      <c r="X171" t="inlineStr">
         <is>
           <t>毒砂の精鉱</t>
         </is>
       </c>
-      <c r="Y168" t="inlineStr">
+      <c r="Y171" t="inlineStr">
         <is>
           <t>정교한 독모래 광석</t>
         </is>
       </c>
-      <c r="Z168" t="inlineStr">
+      <c r="Z171" t="inlineStr">
         <is>
           <t>毒砂精矿</t>
         </is>
       </c>
-      <c r="AA168" t="inlineStr">
+      <c r="AA171" t="inlineStr">
         <is>
           <t>毒砂精礦</t>
         </is>
       </c>
-      <c r="AB168" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="AC168" t="inlineStr">
+      <c r="AB171" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC171" t="inlineStr">
         <is>
           <t>Arsenopyrite Raw Ore</t>
         </is>
       </c>
-      <c r="AD168" t="inlineStr">
+      <c r="AD171" t="inlineStr">
         <is>
           <t>毒砂の原鉱</t>
         </is>
       </c>
-      <c r="AE168" t="inlineStr">
+      <c r="AE171" t="inlineStr">
         <is>
           <t>거친 독모래 광석</t>
         </is>
       </c>
-      <c r="AF168" t="inlineStr">
+      <c r="AF171" t="inlineStr">
         <is>
           <t>毒砂粗矿</t>
         </is>
       </c>
-      <c r="AG168" t="inlineStr">
+      <c r="AG171" t="inlineStr">
         <is>
           <t>毒砂粗礦</t>
         </is>
       </c>
-      <c r="AH168" t="inlineStr">
+      <c r="AH171" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>

</xml_diff>

<commit_message>
GLB 06-26 Hypatia Update
</commit_message>
<xml_diff>
--- a/Sinner_Stuff/dispatch.xlsx
+++ b/Sinner_Stuff/dispatch.xlsx
@@ -26944,86 +26944,86 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1099001</v>
+        <v>1053001</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Dream Interpretation</t>
+          <t>Academic Exchange</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>夢の解析</t>
+          <t>学術交流</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>꿈의 해석</t>
+          <t>학술 교류</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>梦的解析</t>
+          <t>学术交流</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>夢的解析</t>
+          <t>學術交流</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+          <t>The Bureau is planning to organize an internal scientific conference to share cutting-edge developments from the scientific community, and has extended a special invitation to a particular Sinner.</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+          <t>最近、学界の第一線の情報を共有するため、管理局は内部科学交流会の開催を計画しており、特別にとあるコンビクトを招待した。</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+          <t>최근 학계의 최신 정보를 얻기 위해 관리국은 내부 과학 교류회를 열기로 했고, 특별히 한 수감자를 초청했다.</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+          <t>近日，管理局计划组织一次内部科学交流会，分享学界的前沿资讯，特别邀请了某位禁闭者参加。</t>
         </is>
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+          <t>近日，管理局計畫組織一次內部科學交流會，分享學界的最新資訊，特別邀請了某位禁閉者參加。</t>
         </is>
       </c>
       <c r="M171" t="inlineStr">
         <is>
-          <t>Hecate</t>
+          <t>Hypatia</t>
         </is>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>ヘカテー</t>
+          <t>ヒパティア</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
         <is>
-          <t>헤카테</t>
+          <t>히파티아</t>
         </is>
       </c>
       <c r="P171" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>伊帕希娅</t>
         </is>
       </c>
       <c r="Q171" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>伊帕希婭</t>
         </is>
       </c>
       <c r="R171" t="inlineStr"/>
@@ -27033,60 +27033,530 @@
       <c r="V171" t="inlineStr"/>
       <c r="W171" t="inlineStr">
         <is>
+          <t>Arsenopyrite Crystal</t>
+        </is>
+      </c>
+      <c r="X171" t="inlineStr">
+        <is>
+          <t>毒砂結晶</t>
+        </is>
+      </c>
+      <c r="Y171" t="inlineStr">
+        <is>
+          <t>독모래 결정</t>
+        </is>
+      </c>
+      <c r="Z171" t="inlineStr">
+        <is>
+          <t>毒砂晶</t>
+        </is>
+      </c>
+      <c r="AA171" t="inlineStr">
+        <is>
+          <t>毒砂晶</t>
+        </is>
+      </c>
+      <c r="AB171" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC171" t="inlineStr">
+        <is>
           <t>Arsenopyrite Concentrate</t>
         </is>
       </c>
-      <c r="X171" t="inlineStr">
+      <c r="AD171" t="inlineStr">
         <is>
           <t>毒砂の精鉱</t>
         </is>
       </c>
-      <c r="Y171" t="inlineStr">
+      <c r="AE171" t="inlineStr">
         <is>
           <t>정교한 독모래 광석</t>
         </is>
       </c>
-      <c r="Z171" t="inlineStr">
+      <c r="AF171" t="inlineStr">
         <is>
           <t>毒砂精矿</t>
         </is>
       </c>
-      <c r="AA171" t="inlineStr">
+      <c r="AG171" t="inlineStr">
         <is>
           <t>毒砂精礦</t>
         </is>
       </c>
-      <c r="AB171" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="AC171" t="inlineStr">
+      <c r="AH171" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>1053002</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Tomb Raiding Professional</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>盗掘職人</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>도굴 장인</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>倒斗匠人</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>盜墓匠人</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>While patrolling the outskirts of DisCity, the patrol discovered a suspicious pit. The Bureau now needs to send a Sinner with relevant excavation experience to assist with the investigation.</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>パトロール隊がディスシティの外周を巡回中、不審な深い穴を発見した。管理局は現在、調査に協力するため、関連作業の経験を持つコンビクトを派遣する必要がある。</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>순찰대가 디스시티 외곽을 순찰하던 중, 의문스러운 구덩이 하나를 발견했다. 관리국에서 관련 작업 경험이 있는 수감자를 파견해 조사 작업을 도와야 한다.</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>巡逻队于狄斯城外围巡查时发现一处可疑深坑，现需管理局派出一名有相关作业经验的禁闭者协助探查工作。</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>巡邏隊於狄斯城外圍巡查時發現一處可疑深坑，現需管理局派出一名有相關作業經驗的禁閉者協助探查工作。</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>Lysandra</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>リサロ</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>리산드라</t>
+        </is>
+      </c>
+      <c r="P172" t="inlineStr">
+        <is>
+          <t>黎莎洛</t>
+        </is>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>黎莎洛</t>
+        </is>
+      </c>
+      <c r="R172" t="inlineStr"/>
+      <c r="S172" t="inlineStr"/>
+      <c r="T172" t="inlineStr"/>
+      <c r="U172" t="inlineStr"/>
+      <c r="V172" t="inlineStr"/>
+      <c r="W172" t="inlineStr">
+        <is>
+          <t>Arsenopyrite Concentrate</t>
+        </is>
+      </c>
+      <c r="X172" t="inlineStr">
+        <is>
+          <t>毒砂の精鉱</t>
+        </is>
+      </c>
+      <c r="Y172" t="inlineStr">
+        <is>
+          <t>정교한 독모래 광석</t>
+        </is>
+      </c>
+      <c r="Z172" t="inlineStr">
+        <is>
+          <t>毒砂精矿</t>
+        </is>
+      </c>
+      <c r="AA172" t="inlineStr">
+        <is>
+          <t>毒砂精礦</t>
+        </is>
+      </c>
+      <c r="AB172" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC172" t="inlineStr">
         <is>
           <t>Arsenopyrite Raw Ore</t>
         </is>
       </c>
-      <c r="AD171" t="inlineStr">
+      <c r="AD172" t="inlineStr">
         <is>
           <t>毒砂の原鉱</t>
         </is>
       </c>
-      <c r="AE171" t="inlineStr">
+      <c r="AE172" t="inlineStr">
         <is>
           <t>거친 독모래 광석</t>
         </is>
       </c>
-      <c r="AF171" t="inlineStr">
+      <c r="AF172" t="inlineStr">
         <is>
           <t>毒砂粗矿</t>
         </is>
       </c>
-      <c r="AG171" t="inlineStr">
+      <c r="AG172" t="inlineStr">
         <is>
           <t>毒砂粗礦</t>
         </is>
       </c>
-      <c r="AH171" t="inlineStr">
+      <c r="AH172" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>1053003</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>DisCity Appraisal</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>ディス宝物鑑定</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>디스 보물 감정</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>狄斯鉴宝</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>狄斯鑒寶</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>The Public Security Bureau recently confiscated a collection of ancient artifacts contaminated with Mania from the black market. Some fakes are mixed among them, which must be destroyed immediately. They require assistance of several Sinners skilled in artifact and artwork appraisal.</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>最近、治安局は闇市で狂瞳病に汚染された古代美術品を押収した。その中には贋作も混じっており、直接破棄する必要がある。美術品や古代遺物の鑑定に長けたコンビクト数名の協力が必要だ。</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>치안국은 최근 암시장에서 변이에 오염된 고대 예술품을 압수했고, 그중에는 위조품도 섞여 있어 즉시 폐기 조치가 필요하다. 이에 따라 유물 및 예술품 감정에 능숙한 수감자 몇 명의 협조가 필요하다.</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>治安局近日在黑市缴获一批受狂厄污染的古代艺术品，其中混有赝品，需直接销毁，现需几名擅长文物及艺术品鉴定的禁闭者协助工作。</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>治安局近日在黑市繳獲一批受狂厄汙染的古代藝術品，其中混有贗品，需直接銷毀，現需幾名擅長文物及藝術品鑑定的禁閉者協助工作。</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>Lysandra</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>リサロ</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>리산드라</t>
+        </is>
+      </c>
+      <c r="P173" t="inlineStr">
+        <is>
+          <t>黎莎洛</t>
+        </is>
+      </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>黎莎洛</t>
+        </is>
+      </c>
+      <c r="R173" t="inlineStr">
+        <is>
+          <t>McQueen</t>
+        </is>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
+          <t>マックイーン</t>
+        </is>
+      </c>
+      <c r="T173" t="inlineStr">
+        <is>
+          <t>맥퀸</t>
+        </is>
+      </c>
+      <c r="U173" t="inlineStr">
+        <is>
+          <t>麦昆</t>
+        </is>
+      </c>
+      <c r="V173" t="inlineStr">
+        <is>
+          <t>麥昆</t>
+        </is>
+      </c>
+      <c r="W173" t="inlineStr">
+        <is>
+          <t>Arsenopyrite Concentrate</t>
+        </is>
+      </c>
+      <c r="X173" t="inlineStr">
+        <is>
+          <t>毒砂の精鉱</t>
+        </is>
+      </c>
+      <c r="Y173" t="inlineStr">
+        <is>
+          <t>정교한 독모래 광석</t>
+        </is>
+      </c>
+      <c r="Z173" t="inlineStr">
+        <is>
+          <t>毒砂精矿</t>
+        </is>
+      </c>
+      <c r="AA173" t="inlineStr">
+        <is>
+          <t>毒砂精礦</t>
+        </is>
+      </c>
+      <c r="AB173" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC173" t="inlineStr">
+        <is>
+          <t>Arsenopyrite Concentrate</t>
+        </is>
+      </c>
+      <c r="AD173" t="inlineStr">
+        <is>
+          <t>毒砂の精鉱</t>
+        </is>
+      </c>
+      <c r="AE173" t="inlineStr">
+        <is>
+          <t>정교한 독모래 광석</t>
+        </is>
+      </c>
+      <c r="AF173" t="inlineStr">
+        <is>
+          <t>毒砂精矿</t>
+        </is>
+      </c>
+      <c r="AG173" t="inlineStr">
+        <is>
+          <t>毒砂精礦</t>
+        </is>
+      </c>
+      <c r="AH173" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>1099001</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Dream Interpretation</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>夢の解析</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>꿈의 해석</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>梦的解析</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>夢的解析</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>Hecate</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>ヘカテー</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>헤카테</t>
+        </is>
+      </c>
+      <c r="P174" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="R174" t="inlineStr"/>
+      <c r="S174" t="inlineStr"/>
+      <c r="T174" t="inlineStr"/>
+      <c r="U174" t="inlineStr"/>
+      <c r="V174" t="inlineStr"/>
+      <c r="W174" t="inlineStr">
+        <is>
+          <t>Arsenopyrite Concentrate</t>
+        </is>
+      </c>
+      <c r="X174" t="inlineStr">
+        <is>
+          <t>毒砂の精鉱</t>
+        </is>
+      </c>
+      <c r="Y174" t="inlineStr">
+        <is>
+          <t>정교한 독모래 광석</t>
+        </is>
+      </c>
+      <c r="Z174" t="inlineStr">
+        <is>
+          <t>毒砂精矿</t>
+        </is>
+      </c>
+      <c r="AA174" t="inlineStr">
+        <is>
+          <t>毒砂精礦</t>
+        </is>
+      </c>
+      <c r="AB174" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC174" t="inlineStr">
+        <is>
+          <t>Arsenopyrite Raw Ore</t>
+        </is>
+      </c>
+      <c r="AD174" t="inlineStr">
+        <is>
+          <t>毒砂の原鉱</t>
+        </is>
+      </c>
+      <c r="AE174" t="inlineStr">
+        <is>
+          <t>거친 독모래 광석</t>
+        </is>
+      </c>
+      <c r="AF174" t="inlineStr">
+        <is>
+          <t>毒砂粗矿</t>
+        </is>
+      </c>
+      <c r="AG174" t="inlineStr">
+        <is>
+          <t>毒砂粗礦</t>
+        </is>
+      </c>
+      <c r="AH174" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>

</xml_diff>

<commit_message>
GLB Update - Shin Patch
</commit_message>
<xml_diff>
--- a/Sinner_Stuff/dispatch.xlsx
+++ b/Sinner_Stuff/dispatch.xlsx
@@ -553,12 +553,12 @@
       </c>
       <c r="AA1" t="inlineStr">
         <is>
+          <t>Base Reward TW</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
           <t>Base Reward Quantity</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>Base Reward TW</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
@@ -28034,86 +28034,86 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>1099001</v>
+        <v>1055001</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Dream Interpretation</t>
+          <t>Oceanographer</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>夢の解析</t>
+          <t>海洋学者</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>꿈의 해석</t>
+          <t>해양학자</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>梦的解析</t>
+          <t>海洋学家</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>夢的解析</t>
+          <t>海洋學家</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+          <t>Recently, marine animals at the Eastside Aquarium have been dying unnaturally and Mania contamination is suspected to be the cause. The Bureau has been requested to send a Sinner with significant contributions in the marine biology field to assist with the investigation.</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+          <t>最近、ニューシティの水族館で海洋生物が相次いで不審死している。死因は恐らく狂瞳病の汚染だ。海洋生物研究の実績があるコンビクトを研究協力のため派遣をするよう、管理局に申請が届いた。</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+          <t>최근 신성 해양관에서 해양 생물이 연이어 의문사했으며, 사인은 변이 오염과 관련된 것으로 추정한다. 이에 해양관 측은 관리국에 해양 생물을 잘 알고 있는 수감자의 파견을 요청하여 조사 지원을 받고자 한다.</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+          <t>近日，新城海洋馆的海洋生物接连离奇死亡，死因疑似涉及狂厄污染。现特向管理局申请派遣一位对海洋生物研究颇有成果的禁闭者前往协助研究。</t>
         </is>
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+          <t>近日，新城海洋館的海洋生物接連離奇死亡，死因疑似涉及狂厄汙染。現特向管理局申請派遣一位對海洋生物研究頗有成果的禁閉者前往協助研究。</t>
         </is>
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>Hecate</t>
+          <t>Shin</t>
         </is>
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>ヘカテー</t>
+          <t>シズ</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
         <is>
-          <t>헤카테</t>
+          <t>원진</t>
         </is>
       </c>
       <c r="P178" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>源津</t>
         </is>
       </c>
       <c r="Q178" t="inlineStr">
         <is>
-          <t>赫卡蒂</t>
+          <t>源津</t>
         </is>
       </c>
       <c r="R178" t="inlineStr"/>
@@ -28123,60 +28123,530 @@
       <c r="V178" t="inlineStr"/>
       <c r="W178" t="inlineStr">
         <is>
+          <t>Twilight Crystal</t>
+        </is>
+      </c>
+      <c r="X178" t="inlineStr">
+        <is>
+          <t>暮輝結晶</t>
+        </is>
+      </c>
+      <c r="Y178" t="inlineStr">
+        <is>
+          <t>노을 결정</t>
+        </is>
+      </c>
+      <c r="Z178" t="inlineStr">
+        <is>
+          <t>暮辉晶</t>
+        </is>
+      </c>
+      <c r="AA178" t="inlineStr">
+        <is>
+          <t>暮輝晶</t>
+        </is>
+      </c>
+      <c r="AB178" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC178" t="inlineStr">
+        <is>
+          <t>Twilight Stone Concentrate</t>
+        </is>
+      </c>
+      <c r="AD178" t="inlineStr">
+        <is>
+          <t>暮輝石の精鉱</t>
+        </is>
+      </c>
+      <c r="AE178" t="inlineStr">
+        <is>
+          <t>정교한 노을석 광석</t>
+        </is>
+      </c>
+      <c r="AF178" t="inlineStr">
+        <is>
+          <t>暮辉石精矿</t>
+        </is>
+      </c>
+      <c r="AG178" t="inlineStr">
+        <is>
+          <t>暮輝石精礦</t>
+        </is>
+      </c>
+      <c r="AH178" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>1055002</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Dessert Festival</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>スイーツフェス</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>디저트 축제</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>甜品节</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>甜點節</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Ads about the Eastside Dessert Festival are everywhere, claiming to offer unlimited free samples of new desserts! After getting the same ad for the tenth time, a certain Sinner finally gives in and submits an outing application.</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>現在、ニューシティでスイーツフェスが大々的に宣伝されている。なんと新作スイーツが全て無料で試食し放題だという。あるコンビクトは広告を見た回数が10回目に達した時、とうとう我慢できずに管理局に外出申請を出した。</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>신메뉴 디저트를 무료로 무제한 맛볼 수 있는 신성 디저트 축제의 광고가 연일 쏟아졌다. 관련 광고를 벌써 열 번이나 본 어느 수감자는 결국 유혹을 이기지 못해 관리국에 외출을 신청했다.</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>新城甜品节火热宣传中，所有新式甜品免费试吃到饱！第十次刷到相关宣传广告，某位禁闭者终于按耐不住，向管理局提出了外出申请。</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>新城甜點節火熱宣傳中，所有新式甜點免費試吃到飽！第十次看到相關宣傳廣告，某位禁閉者終於按捺不住，向管理局提出了外出申請。</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>Poffy</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>ポフィー</t>
+        </is>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>뽀삐</t>
+        </is>
+      </c>
+      <c r="P179" t="inlineStr">
+        <is>
+          <t>啵啡</t>
+        </is>
+      </c>
+      <c r="Q179" t="inlineStr">
+        <is>
+          <t>啵啡</t>
+        </is>
+      </c>
+      <c r="R179" t="inlineStr"/>
+      <c r="S179" t="inlineStr"/>
+      <c r="T179" t="inlineStr"/>
+      <c r="U179" t="inlineStr"/>
+      <c r="V179" t="inlineStr"/>
+      <c r="W179" t="inlineStr">
+        <is>
+          <t>Twilight Stone Concentrate</t>
+        </is>
+      </c>
+      <c r="X179" t="inlineStr">
+        <is>
+          <t>暮輝石の精鉱</t>
+        </is>
+      </c>
+      <c r="Y179" t="inlineStr">
+        <is>
+          <t>정교한 노을석 광석</t>
+        </is>
+      </c>
+      <c r="Z179" t="inlineStr">
+        <is>
+          <t>暮辉石精矿</t>
+        </is>
+      </c>
+      <c r="AA179" t="inlineStr">
+        <is>
+          <t>暮輝石精礦</t>
+        </is>
+      </c>
+      <c r="AB179" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC179" t="inlineStr">
+        <is>
+          <t>Twilight Stone Raw Ore</t>
+        </is>
+      </c>
+      <c r="AD179" t="inlineStr">
+        <is>
+          <t>暮輝石の原鉱</t>
+        </is>
+      </c>
+      <c r="AE179" t="inlineStr">
+        <is>
+          <t>거친 노을석 광석</t>
+        </is>
+      </c>
+      <c r="AF179" t="inlineStr">
+        <is>
+          <t>暮辉石粗矿</t>
+        </is>
+      </c>
+      <c r="AG179" t="inlineStr">
+        <is>
+          <t>暮輝石粗礦</t>
+        </is>
+      </c>
+      <c r="AH179" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>1055003</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Tasty Visit</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>試食トレンド</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>가게 탐방</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>探店潮流</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>探店潮流</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>A new dessert parlor has recently launched a major online promotional campaign, inviting influencers to sample their products. Having received the invite, both Poffy and Ignis are eager about the tempting offer.</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>最近、ある新しいスイーツ店がネット上で大規模なプロモーションを展開し、多くのインフルエンサーに試食の招待を送っている。招待を受けたポフィーとイグニはどちらも強い興味を示した。</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>최근 한 신흥 디저트 가게가 온라인에서 대대적인 홍보를 진행하며 여러 인플루언서를 초청했다. 초대를 받은 뽀삐와 이그니스 모두 큰 관심을 보였다.</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>近期，某新兴甜品店在网络进行大规模推广，并邀请各路博主前往探店试吃。收到邀请的啵啡和伊格尼都表现出了极大的兴趣。</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>近期，某新興甜點店在網路進行大規模推廣，並邀請各路網紅前往店家試吃。收到邀請的啵啡和伊格尼都表現出了極大的興趣。</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>Poffy</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>ポフィー</t>
+        </is>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>뽀삐</t>
+        </is>
+      </c>
+      <c r="P180" t="inlineStr">
+        <is>
+          <t>啵啡</t>
+        </is>
+      </c>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>啵啡</t>
+        </is>
+      </c>
+      <c r="R180" t="inlineStr">
+        <is>
+          <t>Ignis</t>
+        </is>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
+          <t>イグニ</t>
+        </is>
+      </c>
+      <c r="T180" t="inlineStr">
+        <is>
+          <t>이그니스</t>
+        </is>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
+          <t>伊格尼</t>
+        </is>
+      </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>伊格尼</t>
+        </is>
+      </c>
+      <c r="W180" t="inlineStr">
+        <is>
+          <t>Twilight Stone Concentrate</t>
+        </is>
+      </c>
+      <c r="X180" t="inlineStr">
+        <is>
+          <t>暮輝石の精鉱</t>
+        </is>
+      </c>
+      <c r="Y180" t="inlineStr">
+        <is>
+          <t>정교한 노을석 광석</t>
+        </is>
+      </c>
+      <c r="Z180" t="inlineStr">
+        <is>
+          <t>暮辉石精矿</t>
+        </is>
+      </c>
+      <c r="AA180" t="inlineStr">
+        <is>
+          <t>暮輝石精礦</t>
+        </is>
+      </c>
+      <c r="AB180" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC180" t="inlineStr">
+        <is>
+          <t>Twilight Stone Concentrate</t>
+        </is>
+      </c>
+      <c r="AD180" t="inlineStr">
+        <is>
+          <t>暮輝石の精鉱</t>
+        </is>
+      </c>
+      <c r="AE180" t="inlineStr">
+        <is>
+          <t>정교한 노을석 광석</t>
+        </is>
+      </c>
+      <c r="AF180" t="inlineStr">
+        <is>
+          <t>暮辉石精矿</t>
+        </is>
+      </c>
+      <c r="AG180" t="inlineStr">
+        <is>
+          <t>暮輝石精礦</t>
+        </is>
+      </c>
+      <c r="AH180" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>1099001</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Dream Interpretation</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>夢の解析</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>꿈의 해석</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>梦的解析</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>夢的解析</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Residents in some areas of Eastside often suffer from nightmares. It is necessary to find out why.</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>ニューシティの一部エリアの住民がよくナイトメアにうなされている。具体的な原因を調査しなければならない。</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>신성 일부 지역 주민들은 악몽을 자주꾼다. 구체적인 원인을 철저히 조사해야 한다.</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>新城一些区域的居民经常做噩梦，需要查清具体原因。</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>新城一些區域的居民經常做惡夢，需要查明具體原因。</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>Hecate</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>ヘカテー</t>
+        </is>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>헤카테</t>
+        </is>
+      </c>
+      <c r="P181" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>赫卡蒂</t>
+        </is>
+      </c>
+      <c r="R181" t="inlineStr"/>
+      <c r="S181" t="inlineStr"/>
+      <c r="T181" t="inlineStr"/>
+      <c r="U181" t="inlineStr"/>
+      <c r="V181" t="inlineStr"/>
+      <c r="W181" t="inlineStr">
+        <is>
           <t>Arsenopyrite Concentrate</t>
         </is>
       </c>
-      <c r="X178" t="inlineStr">
+      <c r="X181" t="inlineStr">
         <is>
           <t>毒砂の精鉱</t>
         </is>
       </c>
-      <c r="Y178" t="inlineStr">
+      <c r="Y181" t="inlineStr">
         <is>
           <t>정교한 독모래 광석</t>
         </is>
       </c>
-      <c r="Z178" t="inlineStr">
+      <c r="Z181" t="inlineStr">
         <is>
           <t>毒砂精矿</t>
         </is>
       </c>
-      <c r="AA178" t="inlineStr">
+      <c r="AA181" t="inlineStr">
         <is>
           <t>毒砂精礦</t>
         </is>
       </c>
-      <c r="AB178" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="AC178" t="inlineStr">
+      <c r="AB181" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="AC181" t="inlineStr">
         <is>
           <t>Arsenopyrite Raw Ore</t>
         </is>
       </c>
-      <c r="AD178" t="inlineStr">
+      <c r="AD181" t="inlineStr">
         <is>
           <t>毒砂の原鉱</t>
         </is>
       </c>
-      <c r="AE178" t="inlineStr">
+      <c r="AE181" t="inlineStr">
         <is>
           <t>거친 독모래 광석</t>
         </is>
       </c>
-      <c r="AF178" t="inlineStr">
+      <c r="AF181" t="inlineStr">
         <is>
           <t>毒砂粗矿</t>
         </is>
       </c>
-      <c r="AG178" t="inlineStr">
+      <c r="AG181" t="inlineStr">
         <is>
           <t>毒砂粗礦</t>
         </is>
       </c>
-      <c r="AH178" t="inlineStr">
+      <c r="AH181" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>

</xml_diff>